<commit_message>
write reporting log files
</commit_message>
<xml_diff>
--- a/trapper_data_report.xlsx
+++ b/trapper_data_report.xlsx
@@ -33756,7 +33756,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O68"/>
+  <dimension ref="A1:O70"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -36189,6 +36189,84 @@
       </c>
       <c r="O68" s="2" t="inlineStr"/>
     </row>
+    <row r="69">
+      <c r="A69" s="2" t="inlineStr">
+        <is>
+          <t>FISHER</t>
+        </is>
+      </c>
+      <c r="B69" s="3" t="n">
+        <v>45598</v>
+      </c>
+      <c r="C69" s="2" t="n">
+        <v>51.9487947855414</v>
+      </c>
+      <c r="D69" s="2" t="n">
+        <v>-122.1999941584867</v>
+      </c>
+      <c r="E69" s="2" t="inlineStr">
+        <is>
+          <t>fisher_track_85_photo1.jpg</t>
+        </is>
+      </c>
+      <c r="F69" s="2" t="inlineStr">
+        <is>
+          <t>Not Reviewed</t>
+        </is>
+      </c>
+      <c r="G69" s="2" t="inlineStr"/>
+      <c r="H69" s="2" t="inlineStr"/>
+      <c r="I69" s="2" t="inlineStr"/>
+      <c r="J69" s="2" t="inlineStr"/>
+      <c r="K69" s="2" t="inlineStr"/>
+      <c r="L69" s="2" t="inlineStr"/>
+      <c r="M69" s="2" t="inlineStr"/>
+      <c r="N69" s="2" t="inlineStr">
+        <is>
+          <t>TRACK</t>
+        </is>
+      </c>
+      <c r="O69" s="2" t="inlineStr"/>
+    </row>
+    <row r="70">
+      <c r="A70" s="2" t="inlineStr">
+        <is>
+          <t>FISHER</t>
+        </is>
+      </c>
+      <c r="B70" s="3" t="n">
+        <v>45598</v>
+      </c>
+      <c r="C70" s="2" t="n">
+        <v>51.93205960565463</v>
+      </c>
+      <c r="D70" s="2" t="n">
+        <v>-122.1806457919275</v>
+      </c>
+      <c r="E70" s="2" t="inlineStr">
+        <is>
+          <t>fisher_track_86_photo1.jpg</t>
+        </is>
+      </c>
+      <c r="F70" s="2" t="inlineStr">
+        <is>
+          <t>Not Reviewed</t>
+        </is>
+      </c>
+      <c r="G70" s="2" t="inlineStr"/>
+      <c r="H70" s="2" t="inlineStr"/>
+      <c r="I70" s="2" t="inlineStr"/>
+      <c r="J70" s="2" t="inlineStr"/>
+      <c r="K70" s="2" t="inlineStr"/>
+      <c r="L70" s="2" t="inlineStr"/>
+      <c r="M70" s="2" t="inlineStr"/>
+      <c r="N70" s="2" t="inlineStr">
+        <is>
+          <t>TRACK</t>
+        </is>
+      </c>
+      <c r="O70" s="2" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>